<commit_message>
notebooks and other things
</commit_message>
<xml_diff>
--- a/data/Oman.Tian.2023.xlsx
+++ b/data/Oman.Tian.2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexjames/Desktop/EASM_Regimes/data/new_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deborahkhider/Documents/GitHub/pylipdTutorials/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6960A78-5C3D-1241-B23F-18460365AA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A2D0CC-7D6B-0A44-8D75-63AAF5493563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="940" windowWidth="34560" windowHeight="19840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53040" yWindow="3340" windowWidth="28400" windowHeight="16900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -2557,7 +2557,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A7:I50"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
@@ -3482,8 +3482,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3841,7 +3841,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AB2225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1437" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+    <sheetView topLeftCell="A1437" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
       <selection activeCell="C1443" sqref="C1443"/>
     </sheetView>
   </sheetViews>

</xml_diff>